<commit_message>
Project alert1 is saved.TEST Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/alert1/Main.xlsx
+++ b/DESIGN/rules/alert1/Main.xlsx
@@ -264,6 +264,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -562,7 +563,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -965,18 +966,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="2.85546875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="1" width="5.42578125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="1" width="18.7109375" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="1" width="19.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="1" width="24.28515625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="1" width="25.85546875" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="1" width="11.42578125" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" style="1" width="12.85546875" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="1" width="14.28515625" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="1" width="12.85546875" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="1" width="13.0" collapsed="false"/>
+    <col min="12" max="16384" style="1" width="9.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1071,8 +1072,8 @@
       <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="20">
-        <v>18</v>
+      <c r="C10" s="20" t="n">
+        <v>19.0</v>
       </c>
       <c r="D10" s="21">
         <v>21</v>

</xml_diff>

<commit_message>
Restored from revision #ba2fc01d22c321458b86684e19066dd142eb40f1.TEST Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/alert1/Main.xlsx
+++ b/DESIGN/rules/alert1/Main.xlsx
@@ -264,6 +264,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -562,7 +563,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -965,18 +966,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="2.85546875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="1" width="5.42578125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="1" width="18.7109375" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="1" width="19.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="1" width="24.28515625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="1" width="25.85546875" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="1" width="11.42578125" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" style="1" width="12.85546875" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="1" width="14.28515625" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="1" width="12.85546875" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="1" width="13.0" collapsed="false"/>
+    <col min="12" max="16384" style="1" width="9.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1071,8 +1072,8 @@
       <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="20">
-        <v>18</v>
+      <c r="C10" s="20" t="n">
+        <v>20.0</v>
       </c>
       <c r="D10" s="21">
         <v>21</v>

</xml_diff>

<commit_message>
Restored from revision #10c551cadfdda3faaae334473675be09a8dce4da.TEST Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/alert1/Main.xlsx
+++ b/DESIGN/rules/alert1/Main.xlsx
@@ -264,6 +264,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -562,7 +563,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -965,18 +966,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="2.85546875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="1" width="5.42578125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="1" width="18.7109375" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="1" width="19.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="1" width="24.28515625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="1" width="25.85546875" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="1" width="11.42578125" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" style="1" width="12.85546875" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="1" width="14.28515625" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="1" width="12.85546875" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="1" width="13.0" collapsed="false"/>
+    <col min="12" max="16384" style="1" width="9.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1071,8 +1072,8 @@
       <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="20">
-        <v>18</v>
+      <c r="C10" s="20" t="n">
+        <v>20.0</v>
       </c>
       <c r="D10" s="21">
         <v>21</v>

</xml_diff>

<commit_message>
Restored from revision #132803e0314a84b03ab9ad791cc061ae31c113ec.TEST Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/alert1/Main.xlsx
+++ b/DESIGN/rules/alert1/Main.xlsx
@@ -264,6 +264,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -562,7 +563,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -965,18 +966,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="2.85546875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="1" width="5.42578125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="1" width="18.7109375" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="1" width="19.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="1" width="24.28515625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="1" width="25.85546875" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="1" width="11.42578125" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" style="1" width="12.85546875" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="1" width="14.28515625" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="1" width="12.85546875" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="1" width="13.0" collapsed="false"/>
+    <col min="12" max="16384" style="1" width="9.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1071,8 +1072,8 @@
       <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="20">
-        <v>18</v>
+      <c r="C10" s="20" t="n">
+        <v>20.0</v>
       </c>
       <c r="D10" s="21">
         <v>21</v>

</xml_diff>

<commit_message>
Restored from revision #8105783ef8031ef75e825ea9b34a7e4c2903f2f0.TEST Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/alert1/Main.xlsx
+++ b/DESIGN/rules/alert1/Main.xlsx
@@ -264,6 +264,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -562,7 +563,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -965,18 +966,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="2.85546875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="1" width="5.42578125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="1" width="18.7109375" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="1" width="19.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="1" width="24.28515625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="1" width="25.85546875" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="1" width="11.42578125" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" style="1" width="12.85546875" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="1" width="14.28515625" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="1" width="12.85546875" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="1" width="13.0" collapsed="false"/>
+    <col min="12" max="16384" style="1" width="9.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1071,8 +1072,8 @@
       <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="20">
-        <v>18</v>
+      <c r="C10" s="20" t="n">
+        <v>20.0</v>
       </c>
       <c r="D10" s="21">
         <v>21</v>

</xml_diff>